<commit_message>
Safety Board Automation project
</commit_message>
<xml_diff>
--- a/Output/Inspections Data Mining FSI Analytics.xlsx
+++ b/Output/Inspections Data Mining FSI Analytics.xlsx
@@ -26,156 +26,156 @@
     <t>cwalisso</t>
   </si>
   <si>
+    <t>fnascim</t>
+  </si>
+  <si>
     <t>jhessycc</t>
   </si>
   <si>
-    <t>fnascim</t>
+    <t>nasbeatr</t>
   </si>
   <si>
     <t>limarena</t>
   </si>
   <si>
+    <t>virgrafa</t>
+  </si>
+  <si>
     <t>brunolir</t>
   </si>
   <si>
-    <t>virgrafa</t>
+    <t>sleonr</t>
+  </si>
+  <si>
+    <t>acarolf</t>
   </si>
   <si>
     <t>deanbrun</t>
   </si>
   <si>
+    <t>lucperl</t>
+  </si>
+  <si>
     <t>bjosian</t>
   </si>
   <si>
-    <t>sleonr</t>
-  </si>
-  <si>
     <t>fabcosta</t>
   </si>
   <si>
-    <t>lucperl</t>
-  </si>
-  <si>
-    <t>acarolf</t>
-  </si>
-  <si>
     <t>mrcuama</t>
   </si>
   <si>
-    <t>nasbeatr</t>
+    <t>crmorais</t>
+  </si>
+  <si>
+    <t>elagomes</t>
+  </si>
+  <si>
+    <t>silvkaro</t>
+  </si>
+  <si>
+    <t>gsousa</t>
+  </si>
+  <si>
+    <t>leyls</t>
+  </si>
+  <si>
+    <t>gabriiol</t>
+  </si>
+  <si>
+    <t>visnt</t>
+  </si>
+  <si>
+    <t>olrc</t>
+  </si>
+  <si>
+    <t>anbened</t>
+  </si>
+  <si>
+    <t>alexfeit</t>
+  </si>
+  <si>
+    <t>rodriped</t>
+  </si>
+  <si>
+    <t>pmaicon</t>
+  </si>
+  <si>
+    <t>rafmenez</t>
+  </si>
+  <si>
+    <t>santosev</t>
+  </si>
+  <si>
+    <t>nastiago</t>
+  </si>
+  <si>
+    <t>lmontebe</t>
+  </si>
+  <si>
+    <t>ndasilvi</t>
+  </si>
+  <si>
+    <t>selieni</t>
+  </si>
+  <si>
+    <t>glaannas</t>
+  </si>
+  <si>
+    <t>cavalcaf</t>
+  </si>
+  <si>
+    <t>michatei</t>
+  </si>
+  <si>
+    <t>ariatele</t>
+  </si>
+  <si>
+    <t>ruanasci</t>
+  </si>
+  <si>
+    <t>barivier</t>
+  </si>
+  <si>
+    <t>cadu</t>
+  </si>
+  <si>
+    <t>teidenis</t>
+  </si>
+  <si>
+    <t>tvieira</t>
   </si>
   <si>
     <t>santacam</t>
   </si>
   <si>
+    <t>leaslva</t>
+  </si>
+  <si>
+    <t>vascon</t>
+  </si>
+  <si>
+    <t>eag</t>
+  </si>
+  <si>
+    <t>novaeg</t>
+  </si>
+  <si>
     <t>alvsmarc</t>
   </si>
   <si>
-    <t>barivier</t>
-  </si>
-  <si>
-    <t>leyls</t>
-  </si>
-  <si>
-    <t>ariatele</t>
-  </si>
-  <si>
-    <t>santosev</t>
-  </si>
-  <si>
-    <t>rodriped</t>
-  </si>
-  <si>
-    <t>ruanasci</t>
-  </si>
-  <si>
-    <t>michatei</t>
-  </si>
-  <si>
-    <t>anbened</t>
-  </si>
-  <si>
-    <t>ndasilvi</t>
-  </si>
-  <si>
-    <t>lmontebe</t>
-  </si>
-  <si>
-    <t>vascon</t>
-  </si>
-  <si>
-    <t>selieni</t>
-  </si>
-  <si>
-    <t>elagomes</t>
-  </si>
-  <si>
-    <t>leaslva</t>
-  </si>
-  <si>
-    <t>gabriiol</t>
-  </si>
-  <si>
-    <t>rafmenez</t>
-  </si>
-  <si>
-    <t>visnt</t>
-  </si>
-  <si>
-    <t>alexfeit</t>
-  </si>
-  <si>
-    <t>glaannas</t>
-  </si>
-  <si>
-    <t>novaeg</t>
-  </si>
-  <si>
-    <t>cavalcaf</t>
-  </si>
-  <si>
-    <t>teidenis</t>
-  </si>
-  <si>
-    <t>gsousa</t>
-  </si>
-  <si>
-    <t>crmorais</t>
-  </si>
-  <si>
-    <t>eag</t>
-  </si>
-  <si>
-    <t>tvieira</t>
-  </si>
-  <si>
-    <t>silvkaro</t>
-  </si>
-  <si>
-    <t>nastiago</t>
-  </si>
-  <si>
-    <t>cadu</t>
-  </si>
-  <si>
-    <t>olrc</t>
-  </si>
-  <si>
     <t>fabime</t>
   </si>
   <si>
-    <t>pmaicon</t>
-  </si>
-  <si>
     <t>hzuchina</t>
   </si>
   <si>
+    <t>luivieir</t>
+  </si>
+  <si>
     <t>eniltonm</t>
   </si>
   <si>
-    <t>luivieir</t>
-  </si>
-  <si>
     <t>nisczak</t>
   </si>
   <si>
@@ -197,15 +197,15 @@
     <t>5.06%</t>
   </si>
   <si>
+    <t>Receive</t>
+  </si>
+  <si>
+    <t>4.76%</t>
+  </si>
+  <si>
     <t>Receiving Area</t>
   </si>
   <si>
-    <t>4.76%</t>
-  </si>
-  <si>
-    <t>Receive</t>
-  </si>
-  <si>
     <t>Each Receive</t>
   </si>
   <si>
@@ -248,15 +248,15 @@
     <t>Inbound Dock</t>
   </si>
   <si>
+    <t>Rebin Area</t>
+  </si>
+  <si>
+    <t>1.19%</t>
+  </si>
+  <si>
     <t>PS Area</t>
   </si>
   <si>
-    <t>1.19%</t>
-  </si>
-  <si>
-    <t>Rebin Area</t>
-  </si>
-  <si>
     <t>DANFE</t>
   </si>
   <si>
@@ -269,25 +269,25 @@
     <t>0.48%</t>
   </si>
   <si>
+    <t>Wrangling</t>
+  </si>
+  <si>
+    <t>0.00%</t>
+  </si>
+  <si>
+    <t>Transfer Out</t>
+  </si>
+  <si>
+    <t>Slam</t>
+  </si>
+  <si>
+    <t>PIT/Parking/Charging/Battery Swap</t>
+  </si>
+  <si>
+    <t>Production</t>
+  </si>
+  <si>
     <t>Facilities Engineering</t>
-  </si>
-  <si>
-    <t>0.00%</t>
-  </si>
-  <si>
-    <t>PIT/Parking/Charging/Battery Swap</t>
-  </si>
-  <si>
-    <t>Production</t>
-  </si>
-  <si>
-    <t>Wrangling</t>
-  </si>
-  <si>
-    <t>Transfer Out</t>
-  </si>
-  <si>
-    <t>Slam</t>
   </si>
 </sst>
 </file>
@@ -1101,10 +1101,10 @@
         <v>60</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
         <v>61</v>
@@ -1115,10 +1115,10 @@
         <v>62</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
         <v>61</v>
@@ -1241,10 +1241,10 @@
         <v>77</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D13" t="s">
         <v>78</v>
@@ -1255,10 +1255,10 @@
         <v>79</v>
       </c>
       <c r="B14">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D14" t="s">
         <v>78</v>
@@ -1297,7 +1297,7 @@
         <v>84</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1311,7 +1311,7 @@
         <v>86</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1325,7 +1325,7 @@
         <v>87</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1353,7 +1353,7 @@
         <v>89</v>
       </c>
       <c r="B21">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C21">
         <v>0</v>

</xml_diff>